<commit_message>
#69 Changed two localized sign names.
</commit_message>
<xml_diff>
--- a/database/SQLGenerator.xlsx
+++ b/database/SQLGenerator.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1662,9 +1662,6 @@
     <t>Geben</t>
   </si>
   <si>
-    <t>Weg</t>
-  </si>
-  <si>
     <t>Geh Da Hin</t>
   </si>
   <si>
@@ -1920,9 +1917,6 @@
     <t>Schnell von einer zur anderen Seite</t>
   </si>
   <si>
-    <t>Übergeben</t>
-  </si>
-  <si>
     <t>Gestreckte Zeigefinger aneinander führen</t>
   </si>
   <si>
@@ -1939,6 +1933,12 @@
   </si>
   <si>
     <t>DIN A4-Blatt in die Luft malen</t>
+  </si>
+  <si>
+    <t>Geh weg!</t>
+  </si>
+  <si>
+    <t>Sich übergeben</t>
   </si>
 </sst>
 </file>
@@ -2342,8 +2342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2403,7 +2403,7 @@
         <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -2431,7 +2431,7 @@
         <v>513</v>
       </c>
       <c r="C4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -2475,7 +2475,7 @@
         <v>514</v>
       </c>
       <c r="C6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D6" t="s">
         <v>49</v>
@@ -2519,7 +2519,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D8" t="s">
         <v>49</v>
@@ -2538,7 +2538,7 @@
         <v>489</v>
       </c>
       <c r="B9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C9" t="s">
         <v>140</v>
@@ -2695,7 +2695,7 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D16" t="s">
         <v>49</v>
@@ -2805,7 +2805,7 @@
         <v>520</v>
       </c>
       <c r="C21" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D21" t="s">
         <v>49</v>
@@ -2915,7 +2915,7 @@
         <v>253</v>
       </c>
       <c r="C26" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D26" t="s">
         <v>49</v>
@@ -3289,7 +3289,7 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D43" t="s">
         <v>49</v>
@@ -3333,7 +3333,7 @@
         <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D45" t="s">
         <v>49</v>
@@ -3531,7 +3531,7 @@
         <v>531</v>
       </c>
       <c r="C54" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D54" t="s">
         <v>49</v>
@@ -3553,7 +3553,7 @@
         <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D55" t="s">
         <v>49</v>
@@ -3927,7 +3927,7 @@
         <v>536</v>
       </c>
       <c r="C72" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D72" t="s">
         <v>49</v>
@@ -4276,7 +4276,7 @@
         <v>508</v>
       </c>
       <c r="B88" t="s">
-        <v>545</v>
+        <v>636</v>
       </c>
       <c r="C88" t="s">
         <v>34</v>
@@ -4286,11 +4286,11 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="2"/>
-        <v>insert into signs (name, name_de, mnemonic) values ("go_away","Weg","Wegwerf-Bewegung");</v>
+        <v>insert into signs (name, name_de, mnemonic) values ("go_away","Geh weg!","Wegwerf-Bewegung");</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="3"/>
-        <v>Weg</v>
+        <v>Geh Weg!</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4298,7 +4298,7 @@
         <v>488</v>
       </c>
       <c r="B89" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C89" t="s">
         <v>497</v>
@@ -4342,7 +4342,7 @@
         <v>115</v>
       </c>
       <c r="B91" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C91" t="s">
         <v>44</v>
@@ -4408,7 +4408,7 @@
         <v>437</v>
       </c>
       <c r="B94" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C94" t="s">
         <v>360</v>
@@ -4474,7 +4474,7 @@
         <v>462</v>
       </c>
       <c r="B97" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C97" t="s">
         <v>463</v>
@@ -4518,7 +4518,7 @@
         <v>272</v>
       </c>
       <c r="B99" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C99" t="s">
         <v>202</v>
@@ -4562,10 +4562,10 @@
         <v>494</v>
       </c>
       <c r="B101" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C101" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D101" t="s">
         <v>49</v>
@@ -4606,7 +4606,7 @@
         <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C103" t="s">
         <v>208</v>
@@ -4672,7 +4672,7 @@
         <v>397</v>
       </c>
       <c r="B106" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C106" t="s">
         <v>318</v>
@@ -4738,7 +4738,7 @@
         <v>233</v>
       </c>
       <c r="B109" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C109" t="s">
         <v>158</v>
@@ -4782,7 +4782,7 @@
         <v>471</v>
       </c>
       <c r="B111" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C111" t="s">
         <v>472</v>
@@ -4804,7 +4804,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C112" t="s">
         <v>41</v>
@@ -4826,7 +4826,7 @@
         <v>103</v>
       </c>
       <c r="B113" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C113" t="s">
         <v>102</v>
@@ -4848,10 +4848,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C114" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D114" t="s">
         <v>49</v>
@@ -4914,7 +4914,7 @@
         <v>478</v>
       </c>
       <c r="B117" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C117" t="s">
         <v>357</v>
@@ -4961,7 +4961,7 @@
         <v>19</v>
       </c>
       <c r="C119" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D119" t="s">
         <v>49</v>
@@ -4980,7 +4980,7 @@
         <v>428</v>
       </c>
       <c r="B120" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C120" t="s">
         <v>429</v>
@@ -5024,10 +5024,10 @@
         <v>509</v>
       </c>
       <c r="B122" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C122" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D122" t="s">
         <v>49</v>
@@ -5046,10 +5046,10 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C123" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D123" t="s">
         <v>49</v>
@@ -5090,7 +5090,7 @@
         <v>279</v>
       </c>
       <c r="B125" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C125" t="s">
         <v>281</v>
@@ -5112,7 +5112,7 @@
         <v>481</v>
       </c>
       <c r="B126" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C126" t="s">
         <v>209</v>
@@ -5134,7 +5134,7 @@
         <v>119</v>
       </c>
       <c r="B127" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C127" t="s">
         <v>48</v>
@@ -5178,7 +5178,7 @@
         <v>249</v>
       </c>
       <c r="B129" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C129" t="s">
         <v>179</v>
@@ -5200,7 +5200,7 @@
         <v>460</v>
       </c>
       <c r="B130" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C130" t="s">
         <v>363</v>
@@ -5244,7 +5244,7 @@
         <v>270</v>
       </c>
       <c r="B132" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C132" t="s">
         <v>271</v>
@@ -5313,7 +5313,7 @@
         <v>191</v>
       </c>
       <c r="C135" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D135" t="s">
         <v>49</v>
@@ -5376,7 +5376,7 @@
         <v>439</v>
       </c>
       <c r="B138" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C138" t="s">
         <v>361</v>
@@ -5420,7 +5420,7 @@
         <v>114</v>
       </c>
       <c r="B140" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C140" t="s">
         <v>42</v>
@@ -5442,7 +5442,7 @@
         <v>124</v>
       </c>
       <c r="B141" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C141" t="s">
         <v>52</v>
@@ -5464,7 +5464,7 @@
         <v>412</v>
       </c>
       <c r="B142" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="C142" t="s">
         <v>413</v>
@@ -5474,11 +5474,11 @@
       </c>
       <c r="E142" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic) values ("puke","Übergeben","Den Weg von unten aus Mund heraus");</v>
+        <v>insert into signs (name, name_de, mnemonic) values ("puke","Sich übergeben","Den Weg von unten aus Mund heraus");</v>
       </c>
       <c r="G142" t="str">
         <f t="shared" si="5"/>
-        <v>Übergeben</v>
+        <v>Sich Übergeben</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -5508,7 +5508,7 @@
         <v>264</v>
       </c>
       <c r="B144" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C144" t="s">
         <v>198</v>
@@ -5530,7 +5530,7 @@
         <v>434</v>
       </c>
       <c r="B145" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C145" t="s">
         <v>358</v>
@@ -5596,7 +5596,7 @@
         <v>395</v>
       </c>
       <c r="B148" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C148" t="s">
         <v>317</v>
@@ -5684,7 +5684,7 @@
         <v>259</v>
       </c>
       <c r="B152" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C152" t="s">
         <v>266</v>
@@ -5706,7 +5706,7 @@
         <v>117</v>
       </c>
       <c r="B153" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C153" t="s">
         <v>46</v>
@@ -5728,7 +5728,7 @@
         <v>401</v>
       </c>
       <c r="B154" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C154" t="s">
         <v>323</v>
@@ -5794,7 +5794,7 @@
         <v>110</v>
       </c>
       <c r="B157" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C157" t="s">
         <v>37</v>
@@ -5819,7 +5819,7 @@
         <v>13</v>
       </c>
       <c r="C158" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D158" t="s">
         <v>49</v>
@@ -5838,7 +5838,7 @@
         <v>409</v>
       </c>
       <c r="B159" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C159" t="s">
         <v>338</v>
@@ -5882,7 +5882,7 @@
         <v>106</v>
       </c>
       <c r="B161" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C161" t="s">
         <v>501</v>
@@ -5904,7 +5904,7 @@
         <v>426</v>
       </c>
       <c r="B162" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C162" t="s">
         <v>355</v>
@@ -5926,7 +5926,7 @@
         <v>486</v>
       </c>
       <c r="B163" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C163" t="s">
         <v>57</v>
@@ -5970,7 +5970,7 @@
         <v>104</v>
       </c>
       <c r="B165" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C165" t="s">
         <v>105</v>
@@ -5992,7 +5992,7 @@
         <v>483</v>
       </c>
       <c r="B166" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C166" t="s">
         <v>35</v>
@@ -6058,7 +6058,7 @@
         <v>399</v>
       </c>
       <c r="B169" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C169" t="s">
         <v>320</v>
@@ -6080,7 +6080,7 @@
         <v>487</v>
       </c>
       <c r="B170" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>499</v>
@@ -6102,7 +6102,7 @@
         <v>510</v>
       </c>
       <c r="B171" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C171" t="s">
         <v>58</v>
@@ -6190,7 +6190,7 @@
         <v>485</v>
       </c>
       <c r="B175" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C175" t="s">
         <v>53</v>
@@ -6212,10 +6212,10 @@
         <v>100</v>
       </c>
       <c r="B176" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C176" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D176" t="s">
         <v>49</v>
@@ -6234,7 +6234,7 @@
         <v>265</v>
       </c>
       <c r="B177" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C177" t="s">
         <v>267</v>
@@ -6256,7 +6256,7 @@
         <v>482</v>
       </c>
       <c r="B178" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C178" t="s">
         <v>43</v>
@@ -6278,7 +6278,7 @@
         <v>427</v>
       </c>
       <c r="B179" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C179" t="s">
         <v>356</v>
@@ -6300,7 +6300,7 @@
         <v>448</v>
       </c>
       <c r="B180" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C180" t="s">
         <v>371</v>
@@ -6366,7 +6366,7 @@
         <v>449</v>
       </c>
       <c r="B183" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C183" t="s">
         <v>450</v>
@@ -6476,7 +6476,7 @@
         <v>400</v>
       </c>
       <c r="B188" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C188" t="s">
         <v>321</v>
@@ -6498,7 +6498,7 @@
         <v>242</v>
       </c>
       <c r="B189" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C189" t="s">
         <v>170</v>
@@ -6520,7 +6520,7 @@
         <v>120</v>
       </c>
       <c r="B190" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C190" t="s">
         <v>121</v>
@@ -6542,7 +6542,7 @@
         <v>422</v>
       </c>
       <c r="B191" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C191" t="s">
         <v>353</v>
@@ -6586,7 +6586,7 @@
         <v>394</v>
       </c>
       <c r="B193" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C193" t="s">
         <v>316</v>
@@ -6608,7 +6608,7 @@
         <v>109</v>
       </c>
       <c r="B194" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C194" t="s">
         <v>107</v>
@@ -6652,10 +6652,10 @@
         <v>94</v>
       </c>
       <c r="B196" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C196" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D196" t="s">
         <v>49</v>
@@ -6674,7 +6674,7 @@
         <v>97</v>
       </c>
       <c r="B197" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C197" t="s">
         <v>99</v>
@@ -6696,7 +6696,7 @@
         <v>447</v>
       </c>
       <c r="B198" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C198" t="s">
         <v>370</v>
@@ -6718,7 +6718,7 @@
         <v>96</v>
       </c>
       <c r="B199" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C199" t="s">
         <v>98</v>
@@ -6740,10 +6740,10 @@
         <v>441</v>
       </c>
       <c r="B200" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C200" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D200" t="s">
         <v>49</v>
@@ -6784,7 +6784,7 @@
         <v>276</v>
       </c>
       <c r="B202" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C202" t="s">
         <v>206</v>
@@ -6809,7 +6809,7 @@
         <v>131</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D203" t="s">
         <v>49</v>
@@ -6828,7 +6828,7 @@
         <v>511</v>
       </c>
       <c r="B204" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C204" t="s">
         <v>190</v>
@@ -6850,7 +6850,7 @@
         <v>438</v>
       </c>
       <c r="B205" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C205" t="s">
         <v>359</v>
@@ -6872,7 +6872,7 @@
         <v>122</v>
       </c>
       <c r="B206" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C206" t="s">
         <v>50</v>
@@ -6894,7 +6894,7 @@
         <v>451</v>
       </c>
       <c r="B207" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C207" t="s">
         <v>452</v>
@@ -6938,7 +6938,7 @@
         <v>93</v>
       </c>
       <c r="B209" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C209" t="s">
         <v>10</v>
@@ -6960,7 +6960,7 @@
         <v>490</v>
       </c>
       <c r="B210" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C210" t="s">
         <v>40</v>
@@ -6982,7 +6982,7 @@
         <v>442</v>
       </c>
       <c r="B211" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C211" t="s">
         <v>364</v>

</xml_diff>